<commit_message>
mc_daten hinzugefügt, schneemessungen hinzugefügt, plots für alle quellen fertig
</commit_message>
<xml_diff>
--- a/Data/spring_data/measurement_campaign/sites_ref_manual_measurements.xlsx
+++ b/Data/spring_data/measurement_campaign/sites_ref_manual_measurements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ramunbar/Documents/Master/3_Semester/GITHUB/ETH_MP_Alpine_Water_Springs_Modelling/Data/spring_data/measurement_campaign/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF5D9086-6059-7141-A06A-1445D1405C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F34FA64-45C7-6E4F-B6B6-66109717E0AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="500" windowWidth="24740" windowHeight="16520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="500" windowWidth="24740" windowHeight="16480" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -304,7 +304,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -350,6 +350,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -499,7 +500,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J214"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
+    <sheetView topLeftCell="A79" workbookViewId="0">
       <selection activeCell="A88" sqref="A88:XFD119"/>
     </sheetView>
   </sheetViews>
@@ -7149,11 +7150,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF7A9C5A-6BA1-B342-9A44-264997BB874A}">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="9" max="9" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.15">
@@ -7181,7 +7185,7 @@
       <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="27" t="s">
         <v>8</v>
       </c>
       <c r="J1" t="s">
@@ -8089,7 +8093,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C87130A4-C1C5-3947-BFB4-9C1DF44D8A4F}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>

</xml_diff>